<commit_message>
cleanedup supplxls file and satimge.xlsm. New folder created for gdx res
</commit_message>
<xml_diff>
--- a/suppxls/Scen_NZCO2S-2055.xlsx
+++ b/suppxls/Scen_NZCO2S-2055.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682B340C-6E22-43C4-81E6-5107332AED61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0769C99-CFDF-4D34-B22A-FDC25AA9C27D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0AC21F4E-E9F6-4B4C-837E-642D3D11AAD8}"/>
+    <workbookView xWindow="3795" yWindow="-17910" windowWidth="23835" windowHeight="15255" xr2:uid="{0AC21F4E-E9F6-4B4C-837E-642D3D11AAD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>~TFM_INS</t>
   </si>
@@ -75,6 +75,51 @@
   </si>
   <si>
     <t>CO2S</t>
+  </si>
+  <si>
+    <t>~UC_Sets: R_E: REGION1</t>
+  </si>
+  <si>
+    <t>~UC_Sets: T_E:</t>
+  </si>
+  <si>
+    <t>~UC_T</t>
+  </si>
+  <si>
+    <t>UC_N</t>
+  </si>
+  <si>
+    <t>UC_ATTR</t>
+  </si>
+  <si>
+    <t>Cset_CN</t>
+  </si>
+  <si>
+    <t>LimType</t>
+  </si>
+  <si>
+    <t>UC_COMNET</t>
+  </si>
+  <si>
+    <t>UC_COMNET~RHS</t>
+  </si>
+  <si>
+    <t>UC_RHSRT~2018</t>
+  </si>
+  <si>
+    <t>UC_RHSRT~0</t>
+  </si>
+  <si>
+    <t>COMNET,GROWTH</t>
+  </si>
+  <si>
+    <t>LO</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>UC_Growth_CO2S</t>
   </si>
 </sst>
 </file>
@@ -85,7 +130,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,21 +153,78 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="51"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -131,10 +233,24 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -154,6 +270,911 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CO2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$I$27:$N$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2050</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2051</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2052</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2053</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2054</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2055</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$28:$N$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>123.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>92.8125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>69.609375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ECFE-45D0-BC10-1F911465AD2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="543648527"/>
+        <c:axId val="816355855"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="543648527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="816355855"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="816355855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="543648527"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>109537</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>414337</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC8CC280-1A05-FBE0-E638-603A597277AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Bruno Merven" id="{FEA5A6D4-D241-4D27-A40F-D35D0D02BDD4}" userId="S::01405439@wf.uct.ac.za::c7f06137-2c3b-4c5c-8f38-fe1abbc96860" providerId="AD"/>
@@ -161,9 +1182,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -201,7 +1222,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -307,7 +1328,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -449,7 +1470,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -465,27 +1486,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E162F95E-6986-46BA-A628-7C8DB3D3D747}">
-  <dimension ref="B2:E5"/>
+  <dimension ref="B2:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -499,7 +1524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -513,7 +1538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -525,10 +1550,203 @@
       </c>
       <c r="E5" s="1">
         <v>11925</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G14" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="4" t="str">
+        <f>C4</f>
+        <v>CO2S</v>
+      </c>
+      <c r="E16">
+        <v>2018</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16">
+        <v>100</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <f>-E12</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="4" t="str">
+        <f>D16</f>
+        <v>CO2S</v>
+      </c>
+      <c r="E17">
+        <v>2049</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <f>-E13</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="4" t="str">
+        <f>D17</f>
+        <v>CO2S</v>
+      </c>
+      <c r="E18">
+        <v>2050</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18">
+        <v>0.75</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <f>-E13</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>2050</v>
+      </c>
+      <c r="J27">
+        <v>2051</v>
+      </c>
+      <c r="K27">
+        <v>2052</v>
+      </c>
+      <c r="L27">
+        <v>2053</v>
+      </c>
+      <c r="M27">
+        <v>2054</v>
+      </c>
+      <c r="N27">
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28">
+        <v>220</v>
+      </c>
+      <c r="J28">
+        <f>I28*$I$25</f>
+        <v>165</v>
+      </c>
+      <c r="K28">
+        <f t="shared" ref="K28:M28" si="0">J28*$I$25</f>
+        <v>123.75</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>92.8125</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="0"/>
+        <v>69.609375</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Run definitions and gitignore
</commit_message>
<xml_diff>
--- a/suppxls/Scen_NZCO2S-2055.xlsx
+++ b/suppxls/Scen_NZCO2S-2055.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0769C99-CFDF-4D34-B22A-FDC25AA9C27D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D7163F-ECF6-43E4-9C07-0E16BACFA824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3795" yWindow="-17910" windowWidth="23835" windowHeight="15255" xr2:uid="{0AC21F4E-E9F6-4B4C-837E-642D3D11AAD8}"/>
+    <workbookView xWindow="3120" yWindow="945" windowWidth="23835" windowHeight="15255" xr2:uid="{0AC21F4E-E9F6-4B4C-837E-642D3D11AAD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
   <si>
     <t>~TFM_INS</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>UC_Growth_CO2S</t>
+  </si>
+  <si>
+    <t>UC_Growth_CO2EQS</t>
+  </si>
+  <si>
+    <t>CO2EQS</t>
   </si>
 </sst>
 </file>
@@ -325,7 +331,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$28</c:f>
+              <c:f>Sheet1!$N$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -348,7 +354,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$I$27:$N$27</c:f>
+              <c:f>Sheet1!$O$27:$T$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -375,7 +381,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$28:$N$28</c:f>
+              <c:f>Sheet1!$O$28:$T$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1486,10 +1492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E162F95E-6986-46BA-A628-7C8DB3D3D747}">
-  <dimension ref="B2:N28"/>
+  <dimension ref="B2:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,7 +1636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>21</v>
       </c>
@@ -1661,7 +1667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>21</v>
       </c>
@@ -1692,55 +1698,188 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="G23" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25">
+        <v>2018</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25">
+        <v>100</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
       <c r="I25">
+        <f>-E21</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="4">
+        <v>5</v>
+      </c>
+      <c r="O25">
         <v>0.75</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26">
+        <v>2029</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26">
+        <v>100</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <f>-E22</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27">
+        <v>2030</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
       <c r="I27">
+        <f>-E22</f>
+        <v>0</v>
+      </c>
+      <c r="J27" s="4">
+        <v>5</v>
+      </c>
+      <c r="O27">
         <v>2050</v>
       </c>
-      <c r="J27">
+      <c r="P27">
         <v>2051</v>
       </c>
-      <c r="K27">
+      <c r="Q27">
         <v>2052</v>
       </c>
-      <c r="L27">
+      <c r="R27">
         <v>2053</v>
       </c>
-      <c r="M27">
+      <c r="S27">
         <v>2054</v>
       </c>
-      <c r="N27">
+      <c r="T27">
         <v>2055</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H28" t="s">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="N28" t="s">
         <v>20</v>
       </c>
-      <c r="I28">
+      <c r="O28">
         <v>220</v>
       </c>
-      <c r="J28">
-        <f>I28*$I$25</f>
+      <c r="P28">
+        <f>O28*$O$25</f>
         <v>165</v>
       </c>
-      <c r="K28">
-        <f t="shared" ref="K28:M28" si="0">J28*$I$25</f>
+      <c r="Q28">
+        <f>P28*$O$25</f>
         <v>123.75</v>
       </c>
-      <c r="L28">
-        <f t="shared" si="0"/>
+      <c r="R28">
+        <f>Q28*$O$25</f>
         <v>92.8125</v>
       </c>
-      <c r="M28">
-        <f t="shared" si="0"/>
+      <c r="S28">
+        <f>R28*$O$25</f>
         <v>69.609375</v>
       </c>
-      <c r="N28">
+      <c r="T28">
         <v>0</v>
       </c>
     </row>

</xml_diff>